<commit_message>
fonctionnalite controller utilisateur configuration
</commit_message>
<xml_diff>
--- a/rapport journalier/Rapport_journalier_Nassim.xlsx
+++ b/rapport journalier/Rapport_journalier_Nassim.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="24">
   <si>
     <t xml:space="preserve">DATE : </t>
   </si>
@@ -183,10 +183,39 @@
     <t xml:space="preserve">DATE :  </t>
   </si>
   <si>
-    <t>FUNTIONALITE : reglage des conflits</t>
+    <r>
+      <t xml:space="preserve">FUNTIONALITE : </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>reglage des conflits</t>
+    </r>
   </si>
   <si>
-    <t>FUNTIONALITE : coder les controllers</t>
+    <r>
+      <t xml:space="preserve">FUNTIONALITE : </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>coder les controllers</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t>FUNTIONALITE :</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> finition du code connexion utilisateur avec  l'adresse</t>
+    </r>
+  </si>
+  <si>
+    <t>FUNTIONALITE : finition des controllers utilisateur et commencer les controller de services</t>
   </si>
 </sst>
 </file>
@@ -1331,7 +1360,9 @@
       <c r="B113" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C113" s="3"/>
+      <c r="C113" s="16">
+        <v>44049.0</v>
+      </c>
       <c r="D113" s="3"/>
       <c r="E113" s="4" t="s">
         <v>1</v>
@@ -1345,8 +1376,8 @@
       <c r="J113" s="5"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="B114" s="6" t="s">
-        <v>3</v>
+      <c r="B114" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="J114" s="8"/>
     </row>
@@ -1399,7 +1430,9 @@
       <c r="B123" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C123" s="3"/>
+      <c r="C123" s="16">
+        <v>44054.0</v>
+      </c>
       <c r="D123" s="3"/>
       <c r="E123" s="4" t="s">
         <v>1</v>
@@ -1413,8 +1446,8 @@
       <c r="J123" s="5"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="B124" s="6" t="s">
-        <v>3</v>
+      <c r="B124" s="21" t="s">
+        <v>23</v>
       </c>
       <c r="J124" s="8"/>
     </row>

</xml_diff>

<commit_message>
fonctionnalite controller promotion et structure contrat
</commit_message>
<xml_diff>
--- a/rapport journalier/Rapport_journalier_Nassim.xlsx
+++ b/rapport journalier/Rapport_journalier_Nassim.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="26">
   <si>
     <t xml:space="preserve">DATE : </t>
   </si>
@@ -215,7 +215,36 @@
     </r>
   </si>
   <si>
-    <t>FUNTIONALITE : finition des controllers utilisateur et commencer les controller de services</t>
+    <r>
+      <t xml:space="preserve">FUNTIONALITE : </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>finition des controllers utilisateur et commencer les controller de services</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve">FUNTIONALITE : </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t>finition controller de services et commencer controller planning et promotion</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FUNTIONALITE : </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>terminer les controller promotion et service et commencer le controller de contart et tout ce qui va avec</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1500,7 +1529,9 @@
       <c r="B133" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C133" s="3"/>
+      <c r="C133" s="16">
+        <v>44055.0</v>
+      </c>
       <c r="D133" s="3"/>
       <c r="E133" s="4" t="s">
         <v>1</v>
@@ -1514,8 +1545,8 @@
       <c r="J133" s="5"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="B134" s="6" t="s">
-        <v>3</v>
+      <c r="B134" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="J134" s="8"/>
     </row>
@@ -1568,7 +1599,9 @@
       <c r="B143" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C143" s="3"/>
+      <c r="C143" s="16">
+        <v>44057.0</v>
+      </c>
       <c r="D143" s="3"/>
       <c r="E143" s="4" t="s">
         <v>1</v>
@@ -1582,8 +1615,8 @@
       <c r="J143" s="5"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="B144" s="6" t="s">
-        <v>3</v>
+      <c r="B144" s="21" t="s">
+        <v>25</v>
       </c>
       <c r="J144" s="8"/>
     </row>

</xml_diff>

<commit_message>
fonctionnalites controller utilisateur et photo
</commit_message>
<xml_diff>
--- a/rapport journalier/Rapport_journalier_Nassim.xlsx
+++ b/rapport journalier/Rapport_journalier_Nassim.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="33">
   <si>
     <t xml:space="preserve">DATE : </t>
   </si>
@@ -284,7 +284,7 @@
     </r>
     <r>
       <rPr/>
-      <t>terminer tout les fonctionnalite et commencer le char</t>
+      <t>travailler sur tout les fonctionnalite utilisateur et recherche</t>
     </r>
   </si>
   <si>
@@ -293,8 +293,11 @@
     </r>
     <r>
       <rPr/>
-      <t>terminer les controller promotion et service et commencer le controller de contart et tout ce qui va avec</t>
-    </r>
+      <t>travailler sur tout ce qui est utilisateur et recherche</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">DIFICULTE: </t>
   </si>
   <si>
     <r>
@@ -302,7 +305,7 @@
     </r>
     <r>
       <rPr/>
-      <t>terminer les controller promotion et service et commencer le controller de contart et tout ce qui va avec</t>
+      <t>ajouter quelques fonctionnalite pour controller utilisateur et coder les routes pour les photos</t>
     </r>
   </si>
 </sst>
@@ -410,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -443,6 +446,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1939,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="C183" s="16">
-        <v>44057.0</v>
+        <v>44063.0</v>
       </c>
       <c r="D183" s="3"/>
       <c r="E183" s="4" t="s">
@@ -1968,8 +1974,8 @@
       <c r="J186" s="8"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="B187" s="10" t="s">
-        <v>5</v>
+      <c r="B187" s="22" t="s">
+        <v>31</v>
       </c>
       <c r="C187" s="11"/>
       <c r="D187" s="11"/>
@@ -2009,7 +2015,7 @@
         <v>0</v>
       </c>
       <c r="C193" s="16">
-        <v>44057.0</v>
+        <v>44064.0</v>
       </c>
       <c r="D193" s="3"/>
       <c r="E193" s="4" t="s">
@@ -2025,7 +2031,7 @@
     </row>
     <row r="194" ht="15.75" customHeight="1">
       <c r="B194" s="21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J194" s="8"/>
     </row>

</xml_diff>